<commit_message>
getting chart to work and styling the home page
</commit_message>
<xml_diff>
--- a/data/freddieMac.xlsx
+++ b/data/freddieMac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelTanner\Documents\code_doc\java\redashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BC85306-FD7D-4934-B0F6-09DA71F7C079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817A7643-AF28-4349-AD34-DDABBFE98CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="2370" windowWidth="21600" windowHeight="11295" xr2:uid="{85C5DE01-2C0E-49AE-AF1A-B3DD65461ECA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85C5DE01-2C0E-49AE-AF1A-B3DD65461ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,20 +47,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Helv"/>
     </font>
     <font>
       <sz val="11"/>
@@ -92,16 +85,16 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -420,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EF6ABD-431C-421F-B0DE-896A24D06EA1}">
   <dimension ref="A1:B2650"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>